<commit_message>
Updated README.md in include React component momemt.  Also cleaned up ProductCategoryTable.js for variables showing not used
</commit_message>
<xml_diff>
--- a/ProjectFiles/Documentation/Project2-SystemOverview.xlsx
+++ b/ProjectFiles/Documentation/Project2-SystemOverview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EvolveU\Project2\POS\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EvolveU\Project2\POS\ProjectFiles\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F13C39-642A-49CC-B795-870CA1E106F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0DD199-9848-42A4-828B-85DCE0B491BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -1713,7 +1713,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- active</a:t>
+            <a:t>- status</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -3621,6 +3621,110 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>581026</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="TextBox 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC09FBDC-84AE-4E8D-83FC-D680C2907F7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9115426" y="4914900"/>
+          <a:ext cx="2495550" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>Note:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>- For Order - Status</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>- Created</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>- Filled</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>- Shipped</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>- Completed</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3892,13 +3996,14 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="AD28" sqref="AD28"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Modified user.json changed accessLevel to userLevel, added orderStatus.json, modified order.json to include orderStatus data
</commit_message>
<xml_diff>
--- a/ProjectFiles/Documentation/Project2-SystemOverview.xlsx
+++ b/ProjectFiles/Documentation/Project2-SystemOverview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EvolveU\Project2\POS\ProjectFiles\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0DD199-9848-42A4-828B-85DCE0B491BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BEA358-06AE-4D6B-9291-14E7095061B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2488,7 +2488,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>- levelId</a:t>
+            <a:t>- UserLevel</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -3995,7 +3995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
       <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update Project Overview document. Created new set of test data.
</commit_message>
<xml_diff>
--- a/ProjectFiles/Documentation/Project2-SystemOverview.xlsx
+++ b/ProjectFiles/Documentation/Project2-SystemOverview.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EvolveU\Project2\POS\ProjectFiles\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BEA358-06AE-4D6B-9291-14E7095061B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09105447-EE9E-46F2-9A62-EF23825D0E8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Tables" sheetId="2" r:id="rId2"/>
+    <sheet name="Scope" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,6 +24,107 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+  <si>
+    <t>Phase 1</t>
+  </si>
+  <si>
+    <t>Develop application lookup maintenance forms:</t>
+  </si>
+  <si>
+    <t>Develop application main forms:</t>
+  </si>
+  <si>
+    <t>User maintenance</t>
+  </si>
+  <si>
+    <t>User Level maintenance</t>
+  </si>
+  <si>
+    <t>Order Status maintenance</t>
+  </si>
+  <si>
+    <t>Product Category maintenance</t>
+  </si>
+  <si>
+    <t>Customer maintenance</t>
+  </si>
+  <si>
+    <t>Product maintenance</t>
+  </si>
+  <si>
+    <t>Supplier maintenance</t>
+  </si>
+  <si>
+    <t>Other tables</t>
+  </si>
+  <si>
+    <t>GST table - for now, embedded in Customer table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Develop </t>
+  </si>
+  <si>
+    <t>Order entry form</t>
+  </si>
+  <si>
+    <t>Login form</t>
+  </si>
+  <si>
+    <t>Inventory maintenance</t>
+  </si>
+  <si>
+    <t>Order processing form</t>
+  </si>
+  <si>
+    <t>Order processing backend</t>
+  </si>
+  <si>
+    <t>Phase 3</t>
+  </si>
+  <si>
+    <t>Develop remote order sync/upload to main database process</t>
+  </si>
+  <si>
+    <t>This might require additional columns in the main database, orders table, for keeping track of status of sync/upload</t>
+  </si>
+  <si>
+    <t>Develop data sync from main database to remote units</t>
+  </si>
+  <si>
+    <t>This process is for refreshing data in remote units.  Example, new customer created by admin in main database.</t>
+  </si>
+  <si>
+    <t>new products created by admin in main database.</t>
+  </si>
+  <si>
+    <t>and possibly other type of data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate invoice paper </t>
+  </si>
+  <si>
+    <t>Generate order paper/pdf form</t>
+  </si>
+  <si>
+    <t>Develop functionality to send pdf order form to customer via email, from remote or backoffice</t>
+  </si>
+  <si>
+    <t>This form is for order fulfillment, shipping order</t>
+  </si>
+  <si>
+    <t>This will be responsible for updating inventory based on order once fulfilled</t>
+  </si>
+  <si>
+    <t>Generate order fulfillment checklist</t>
+  </si>
+  <si>
+    <t>This form is for updating product inventory as  products are received for top up.  Order count adjustment process, etc.</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -36,12 +138,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -56,8 +164,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3995,8 +4104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4017,4 +4126,170 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E579ABFE-F91A-4469-9534-1B8E0434E592}">
+  <dimension ref="B2:P36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>19</v>
+      </c>
+      <c r="J33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>21</v>
+      </c>
+      <c r="J34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="P35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="P36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated test data and System overview document
</commit_message>
<xml_diff>
--- a/ProjectFiles/Documentation/Project2-SystemOverview.xlsx
+++ b/ProjectFiles/Documentation/Project2-SystemOverview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EvolveU\Project2\POS\ProjectFiles\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F0D330-AAC6-44FA-8BD3-29716EF52396}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598D0301-D3E5-4C19-8FA4-C1366FB718BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Phase 1</t>
   </si>
@@ -127,15 +127,34 @@
   <si>
     <t>Develop dashboard type screen for quick overview of what is happening in the system</t>
   </si>
+  <si>
+    <t>Phase 2</t>
+  </si>
+  <si>
+    <t>Modernize application frontend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extra </t>
+  </si>
+  <si>
+    <t>Put something in the Home page????</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -173,10 +192,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4154,7 +4174,7 @@
   <dimension ref="B2:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4186,7 +4206,7 @@
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4216,13 +4236,21 @@
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>0</v>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -4232,22 +4260,22 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -4272,6 +4300,11 @@
       </c>
       <c r="H26" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -4317,5 +4350,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>